<commit_message>
- IOMPshift.py, IOMPshift_computer.py, MonitoringShift.xlsx; naming
</commit_message>
<xml_diff>
--- a/MonitoringShift.xlsx
+++ b/MonitoringShift.xlsx
@@ -26,133 +26,133 @@
     <t>IOMP-CT</t>
   </si>
   <si>
+    <t>Arnel</t>
+  </si>
+  <si>
+    <t>Junsat</t>
+  </si>
+  <si>
+    <t>Carlo</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Meryll</t>
+  </si>
+  <si>
+    <t>Cath</t>
+  </si>
+  <si>
+    <t>Brain</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>TinB</t>
+  </si>
+  <si>
+    <t>Rodney</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>Earl</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Kennex</t>
+  </si>
+  <si>
+    <t>Biboy</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Marj</t>
+  </si>
+  <si>
+    <t>Zhey</t>
+  </si>
+  <si>
     <t>Prado</t>
   </si>
   <si>
-    <t>Ivy</t>
+    <t>Mart</t>
+  </si>
+  <si>
+    <t>Sky</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Roy</t>
   </si>
   <si>
     <t>Nathan</t>
   </si>
   <si>
-    <t>Meryll</t>
-  </si>
-  <si>
-    <t>Roy</t>
-  </si>
-  <si>
-    <t>TinB</t>
-  </si>
-  <si>
-    <t>Cath</t>
-  </si>
-  <si>
-    <t>Rodney</t>
+    <t>Anj</t>
   </si>
   <si>
     <t>Reyn</t>
   </si>
   <si>
-    <t>Arnel</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Mart</t>
-  </si>
-  <si>
-    <t>Brain</t>
-  </si>
-  <si>
-    <t>Junsat</t>
-  </si>
-  <si>
-    <t>Anj</t>
-  </si>
-  <si>
-    <t>Zhey</t>
-  </si>
-  <si>
-    <t>Marj</t>
-  </si>
-  <si>
-    <t>Carlo</t>
+    <t>Jec</t>
   </si>
   <si>
     <t>Morgan</t>
   </si>
   <si>
-    <t>Biboy</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Jec</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Kennex</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Kate</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Earl</t>
-  </si>
-  <si>
-    <t>Sky</t>
+    <t>Edch</t>
+  </si>
+  <si>
+    <t>Lem</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Ardeth</t>
   </si>
   <si>
     <t>Momay</t>
   </si>
   <si>
+    <t>Pau</t>
+  </si>
+  <si>
+    <t>Daisy</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
     <t>TinC</t>
   </si>
   <si>
     <t>Claud</t>
   </si>
   <si>
-    <t>Anne</t>
-  </si>
-  <si>
-    <t>Daisy</t>
-  </si>
-  <si>
-    <t>Ardeth</t>
-  </si>
-  <si>
     <t>Pati</t>
   </si>
   <si>
-    <t>Harry</t>
-  </si>
-  <si>
     <t>Mikee</t>
   </si>
   <si>
-    <t>Pau</t>
-  </si>
-  <si>
-    <t>Edch</t>
-  </si>
-  <si>
     <t>Eunice</t>
-  </si>
-  <si>
-    <t>Amy</t>
-  </si>
-  <si>
-    <t>Lem</t>
   </si>
   <si>
     <t>Tinb</t>
@@ -548,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -559,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -570,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -581,7 +581,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -592,7 +592,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -603,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -614,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -625,7 +625,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -636,7 +636,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -647,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -658,7 +658,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -669,7 +669,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -680,7 +680,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -691,7 +691,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -702,7 +702,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -713,7 +713,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -724,7 +724,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -735,7 +735,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -746,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -757,7 +757,7 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -768,7 +768,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -779,7 +779,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -790,7 +790,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -801,7 +801,7 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -812,7 +812,7 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -823,7 +823,7 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -834,7 +834,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -845,7 +845,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -856,7 +856,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -864,10 +864,10 @@
         <v>42809.8125</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -875,7 +875,7 @@
         <v>42810.3125</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
         <v>44</v>
@@ -886,7 +886,7 @@
         <v>42810.8125</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>45</v>
@@ -897,10 +897,10 @@
         <v>42811.3125</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -908,10 +908,10 @@
         <v>42811.8125</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -919,10 +919,10 @@
         <v>42812.3125</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -930,10 +930,10 @@
         <v>42812.8125</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -941,10 +941,10 @@
         <v>42813.3125</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -952,10 +952,10 @@
         <v>42813.8125</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -963,10 +963,10 @@
         <v>42814.3125</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -974,10 +974,10 @@
         <v>42814.8125</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -985,10 +985,10 @@
         <v>42815.3125</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -996,10 +996,10 @@
         <v>42815.8125</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>42816.3125</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1021,7 +1021,7 @@
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>42817.3125</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>42817.8125</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>42818.3125</v>
       </c>
       <c r="B48" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>42818.8125</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1073,10 +1073,10 @@
         <v>42819.3125</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1084,10 +1084,10 @@
         <v>42819.8125</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1098,7 +1098,7 @@
         <v>28</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>42820.8125</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>42821.3125</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1128,7 +1128,7 @@
         <v>42821.8125</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -1139,10 +1139,10 @@
         <v>42822.3125</v>
       </c>
       <c r="B56" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1150,10 +1150,10 @@
         <v>42822.8125</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1161,10 +1161,10 @@
         <v>42823.3125</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1172,10 +1172,10 @@
         <v>42823.8125</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1183,10 +1183,10 @@
         <v>42824.3125</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1194,10 +1194,10 @@
         <v>42824.8125</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1205,10 +1205,10 @@
         <v>42825.3125</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C62" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1216,10 +1216,10 @@
         <v>42825.8125</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1254,10 +1254,10 @@
         <v>42767.3125</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1265,10 +1265,10 @@
         <v>42767.8125</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1276,10 +1276,10 @@
         <v>42768.3125</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1287,10 +1287,10 @@
         <v>42768.8125</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1298,10 +1298,10 @@
         <v>42769.3125</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1309,10 +1309,10 @@
         <v>42769.8125</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1320,10 +1320,10 @@
         <v>42770.3125</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1331,10 +1331,10 @@
         <v>42770.8125</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1342,10 +1342,10 @@
         <v>42771.3125</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1353,10 +1353,10 @@
         <v>42771.8125</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1364,10 +1364,10 @@
         <v>42772.3125</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1375,10 +1375,10 @@
         <v>42772.8125</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1389,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1397,10 +1397,10 @@
         <v>42773.8125</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1408,10 +1408,10 @@
         <v>42774.3125</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1419,10 +1419,10 @@
         <v>42774.8125</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1430,10 +1430,10 @@
         <v>42775.3125</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1441,10 +1441,10 @@
         <v>42775.8125</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1452,10 +1452,10 @@
         <v>42776.3125</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1474,10 +1474,10 @@
         <v>42777.3125</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1485,10 +1485,10 @@
         <v>42777.8125</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1496,10 +1496,10 @@
         <v>42778.3125</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1507,7 +1507,7 @@
         <v>42778.8125</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
@@ -1518,10 +1518,10 @@
         <v>42779.3125</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1529,10 +1529,10 @@
         <v>42779.8125</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1540,10 +1540,10 @@
         <v>42780.3125</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1551,10 +1551,10 @@
         <v>42780.8125</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1562,10 +1562,10 @@
         <v>42781.3125</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1573,10 +1573,10 @@
         <v>42781.8125</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1584,10 +1584,10 @@
         <v>42782.3125</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1595,10 +1595,10 @@
         <v>42782.8125</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1606,10 +1606,10 @@
         <v>42783.3125</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1617,10 +1617,10 @@
         <v>42783.8125</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1628,10 +1628,10 @@
         <v>42784.3125</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1642,7 +1642,7 @@
         <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1650,10 +1650,10 @@
         <v>42785.3125</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1661,10 +1661,10 @@
         <v>42785.8125</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1672,10 +1672,10 @@
         <v>42786.3125</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1683,10 +1683,10 @@
         <v>42786.8125</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1694,10 +1694,10 @@
         <v>42787.3125</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1705,10 +1705,10 @@
         <v>42787.8125</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1716,10 +1716,10 @@
         <v>42788.3125</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1727,10 +1727,10 @@
         <v>42788.8125</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1738,10 +1738,10 @@
         <v>42789.3125</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1749,10 +1749,10 @@
         <v>42789.8125</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1760,10 +1760,10 @@
         <v>42790.3125</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1771,10 +1771,10 @@
         <v>42790.8125</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1782,10 +1782,10 @@
         <v>42791.3125</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1793,10 +1793,10 @@
         <v>42791.8125</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1804,10 +1804,10 @@
         <v>42792.3125</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1815,7 +1815,7 @@
         <v>42792.8125</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
         <v>13</v>
@@ -1826,10 +1826,10 @@
         <v>42793.3125</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1837,10 +1837,10 @@
         <v>42793.8125</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1848,7 +1848,7 @@
         <v>42794.3125</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C56" t="s">
         <v>47</v>
@@ -1859,10 +1859,10 @@
         <v>42794.8125</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>